<commit_message>
GeoMap in proxidrugs_py updated
</commit_message>
<xml_diff>
--- a/data/location.xlsx
+++ b/data/location.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reagon.karki\Documents\GitHub\datascience_toolkit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B29CC58-AC81-4E56-B2B7-5EFBE2343F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CE1525-59D8-49C1-B7BD-D3AB2D5AD7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>AbbVie Deutschland</t>
   </si>
@@ -70,6 +79,12 @@
   </si>
   <si>
     <t>München</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
   </si>
 </sst>
 </file>
@@ -395,126 +410,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>6</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="E11">
+        <f>SUM(E2:E10)</f>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>